<commit_message>
updated a university and a name
</commit_message>
<xml_diff>
--- a/rentals.xlsx
+++ b/rentals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\black\Documents\School\DS401COLCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC20C22-5C6C-4383-B77C-5913785C3940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B77C7E-4342-416E-9B0C-9D3C1F2FD405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apartment Prices Granular" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>SUNY College of Technology at Alfred</t>
   </si>
@@ -1457,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:GO43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GL7" workbookViewId="0">
-      <selection activeCell="GQ19" sqref="GQ19:GU34"/>
+    <sheetView tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
+      <selection activeCell="DD11" sqref="DD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,7 +1633,6 @@
     <col min="168" max="168" width="34.109375" bestFit="1" customWidth="1"/>
     <col min="169" max="169" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="170" max="170" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="172" max="172" width="24" bestFit="1" customWidth="1"/>
     <col min="173" max="173" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="174" max="174" width="32.109375" bestFit="1" customWidth="1"/>
@@ -2170,9 +2169,6 @@
       <c r="FN1" t="s">
         <v>169</v>
       </c>
-      <c r="FO1" t="s">
-        <v>170</v>
-      </c>
       <c r="FP1" t="s">
         <v>171</v>
       </c>
@@ -2763,9 +2759,6 @@
       <c r="FN2">
         <v>1282</v>
       </c>
-      <c r="FO2">
-        <v>1669</v>
-      </c>
       <c r="FP2">
         <v>1419</v>
       </c>
@@ -3356,9 +3349,6 @@
       <c r="FN3">
         <v>1144</v>
       </c>
-      <c r="FO3">
-        <v>1561.5</v>
-      </c>
       <c r="FP3">
         <v>1510</v>
       </c>
@@ -3949,9 +3939,6 @@
       <c r="FN4">
         <v>1098.5</v>
       </c>
-      <c r="FO4">
-        <v>1324</v>
-      </c>
       <c r="FP4">
         <v>907</v>
       </c>
@@ -4542,9 +4529,6 @@
       <c r="FN5">
         <v>1129</v>
       </c>
-      <c r="FO5">
-        <v>1280</v>
-      </c>
       <c r="FP5">
         <v>916.5</v>
       </c>
@@ -5135,9 +5119,6 @@
       <c r="FN6">
         <v>1350</v>
       </c>
-      <c r="FO6">
-        <v>1436.5</v>
-      </c>
       <c r="FP6">
         <v>740</v>
       </c>
@@ -5728,9 +5709,6 @@
       <c r="FN7">
         <v>1119.5</v>
       </c>
-      <c r="FO7">
-        <v>1755</v>
-      </c>
       <c r="FP7">
         <v>785</v>
       </c>
@@ -6321,9 +6299,6 @@
       <c r="FN8">
         <v>1250</v>
       </c>
-      <c r="FO8">
-        <v>1421.5</v>
-      </c>
       <c r="FP8">
         <v>0</v>
       </c>
@@ -6914,9 +6889,6 @@
       <c r="FN9">
         <v>790</v>
       </c>
-      <c r="FO9">
-        <v>975</v>
-      </c>
       <c r="FP9">
         <v>0</v>
       </c>
@@ -7507,9 +7479,6 @@
       <c r="FN10">
         <v>665</v>
       </c>
-      <c r="FO10">
-        <v>1326.5</v>
-      </c>
       <c r="FP10">
         <v>0</v>
       </c>
@@ -8100,9 +8069,6 @@
       <c r="FN11">
         <v>700</v>
       </c>
-      <c r="FO11">
-        <v>1385</v>
-      </c>
       <c r="FP11">
         <v>0</v>
       </c>
@@ -8693,9 +8659,6 @@
       <c r="FN12">
         <v>714.5</v>
       </c>
-      <c r="FO12">
-        <v>1374.5</v>
-      </c>
       <c r="FP12">
         <v>0</v>
       </c>
@@ -9286,9 +9249,6 @@
       <c r="FN13">
         <v>725</v>
       </c>
-      <c r="FO13">
-        <v>1268.5</v>
-      </c>
       <c r="FP13">
         <v>0</v>
       </c>
@@ -9879,9 +9839,6 @@
       <c r="FN14">
         <v>612.5</v>
       </c>
-      <c r="FO14">
-        <v>1459</v>
-      </c>
       <c r="FP14">
         <v>0</v>
       </c>
@@ -10472,9 +10429,6 @@
       <c r="FN15">
         <v>0</v>
       </c>
-      <c r="FO15">
-        <v>1237.5</v>
-      </c>
       <c r="FP15">
         <v>0</v>
       </c>
@@ -11065,9 +11019,6 @@
       <c r="FN16">
         <v>0</v>
       </c>
-      <c r="FO16">
-        <v>1552.5</v>
-      </c>
       <c r="FP16">
         <v>0</v>
       </c>
@@ -11658,9 +11609,6 @@
       <c r="FN17">
         <v>0</v>
       </c>
-      <c r="FO17">
-        <v>1237.5</v>
-      </c>
       <c r="FP17">
         <v>0</v>
       </c>
@@ -12251,9 +12199,6 @@
       <c r="FN18">
         <v>0</v>
       </c>
-      <c r="FO18">
-        <v>1082</v>
-      </c>
       <c r="FP18">
         <v>0</v>
       </c>
@@ -12844,9 +12789,6 @@
       <c r="FN19">
         <v>0</v>
       </c>
-      <c r="FO19">
-        <v>1000</v>
-      </c>
       <c r="FP19">
         <v>0</v>
       </c>
@@ -13437,9 +13379,6 @@
       <c r="FN20">
         <v>0</v>
       </c>
-      <c r="FO20">
-        <v>1297.5</v>
-      </c>
       <c r="FP20">
         <v>0</v>
       </c>
@@ -14030,9 +13969,6 @@
       <c r="FN21">
         <v>0</v>
       </c>
-      <c r="FO21">
-        <v>1025</v>
-      </c>
       <c r="FP21">
         <v>0</v>
       </c>
@@ -14623,9 +14559,6 @@
       <c r="FN22">
         <v>0</v>
       </c>
-      <c r="FO22">
-        <v>1025</v>
-      </c>
       <c r="FP22">
         <v>0</v>
       </c>
@@ -15216,9 +15149,6 @@
       <c r="FN23">
         <v>0</v>
       </c>
-      <c r="FO23">
-        <v>1115</v>
-      </c>
       <c r="FP23">
         <v>0</v>
       </c>
@@ -15809,9 +15739,6 @@
       <c r="FN24">
         <v>0</v>
       </c>
-      <c r="FO24">
-        <v>0</v>
-      </c>
       <c r="FP24">
         <v>0</v>
       </c>
@@ -16402,9 +16329,6 @@
       <c r="FN25">
         <v>0</v>
       </c>
-      <c r="FO25">
-        <v>0</v>
-      </c>
       <c r="FP25">
         <v>0</v>
       </c>
@@ -16995,9 +16919,6 @@
       <c r="FN26">
         <v>0</v>
       </c>
-      <c r="FO26">
-        <v>0</v>
-      </c>
       <c r="FP26">
         <v>0</v>
       </c>
@@ -17588,9 +17509,6 @@
       <c r="FN27">
         <v>0</v>
       </c>
-      <c r="FO27">
-        <v>0</v>
-      </c>
       <c r="FP27">
         <v>0</v>
       </c>
@@ -18181,9 +18099,6 @@
       <c r="FN28">
         <v>0</v>
       </c>
-      <c r="FO28">
-        <v>0</v>
-      </c>
       <c r="FP28">
         <v>0</v>
       </c>
@@ -18774,9 +18689,6 @@
       <c r="FN29">
         <v>0</v>
       </c>
-      <c r="FO29">
-        <v>0</v>
-      </c>
       <c r="FP29">
         <v>0</v>
       </c>
@@ -19367,9 +19279,6 @@
       <c r="FN30">
         <v>0</v>
       </c>
-      <c r="FO30">
-        <v>0</v>
-      </c>
       <c r="FP30">
         <v>0</v>
       </c>
@@ -19960,9 +19869,6 @@
       <c r="FN31">
         <v>0</v>
       </c>
-      <c r="FO31">
-        <v>0</v>
-      </c>
       <c r="FP31">
         <v>0</v>
       </c>
@@ -20553,9 +20459,6 @@
       <c r="FN32">
         <v>0</v>
       </c>
-      <c r="FO32">
-        <v>0</v>
-      </c>
       <c r="FP32">
         <v>0</v>
       </c>
@@ -21146,9 +21049,6 @@
       <c r="FN33">
         <v>0</v>
       </c>
-      <c r="FO33">
-        <v>0</v>
-      </c>
       <c r="FP33">
         <v>0</v>
       </c>
@@ -21739,9 +21639,6 @@
       <c r="FN34">
         <v>0</v>
       </c>
-      <c r="FO34">
-        <v>0</v>
-      </c>
       <c r="FP34">
         <v>0</v>
       </c>
@@ -22332,9 +22229,6 @@
       <c r="FN35">
         <v>0</v>
       </c>
-      <c r="FO35">
-        <v>0</v>
-      </c>
       <c r="FP35">
         <v>0</v>
       </c>
@@ -22925,9 +22819,6 @@
       <c r="FN36">
         <v>0</v>
       </c>
-      <c r="FO36">
-        <v>0</v>
-      </c>
       <c r="FP36">
         <v>0</v>
       </c>
@@ -23518,9 +23409,6 @@
       <c r="FN37">
         <v>0</v>
       </c>
-      <c r="FO37">
-        <v>0</v>
-      </c>
       <c r="FP37">
         <v>0</v>
       </c>
@@ -24111,9 +23999,6 @@
       <c r="FN38">
         <v>0</v>
       </c>
-      <c r="FO38">
-        <v>0</v>
-      </c>
       <c r="FP38">
         <v>0</v>
       </c>
@@ -24704,9 +24589,6 @@
       <c r="FN39">
         <v>0</v>
       </c>
-      <c r="FO39">
-        <v>0</v>
-      </c>
       <c r="FP39">
         <v>0</v>
       </c>
@@ -25297,9 +25179,6 @@
       <c r="FN40">
         <v>0</v>
       </c>
-      <c r="FO40">
-        <v>0</v>
-      </c>
       <c r="FP40">
         <v>0</v>
       </c>
@@ -25890,9 +25769,6 @@
       <c r="FN41">
         <v>0</v>
       </c>
-      <c r="FO41">
-        <v>0</v>
-      </c>
       <c r="FP41">
         <v>0</v>
       </c>
@@ -26483,9 +26359,6 @@
       <c r="FN42">
         <v>0</v>
       </c>
-      <c r="FO42">
-        <v>0</v>
-      </c>
       <c r="FP42">
         <v>0</v>
       </c>
@@ -27074,9 +26947,6 @@
         <v>0</v>
       </c>
       <c r="FN43">
-        <v>0</v>
-      </c>
-      <c r="FO43">
         <v>0</v>
       </c>
       <c r="FP43">

</xml_diff>